<commit_message>
Wired all keyboard matrix pins
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver\Documents\GitHub\65-Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9373F5-AC9A-4ABC-A35C-A8FA35D723A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695D610D-8A37-4D3D-9445-BA61B9ED9040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{9889003C-2723-49A8-808D-023C4202CB02}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{9889003C-2723-49A8-808D-023C4202CB02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t>Item #</t>
   </si>
@@ -210,6 +210,21 @@
   </si>
   <si>
     <t>TDFN-8</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U3</t>
   </si>
 </sst>
 </file>
@@ -591,7 +606,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +659,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -673,6 +691,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
       <c r="C3">
         <v>1</v>
       </c>
@@ -745,6 +766,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
       <c r="C6">
         <v>1</v>
       </c>
@@ -787,7 +811,7 @@
         <v>32</v>
       </c>
       <c r="H7" t="str">
-        <f>"0"&amp;603</f>
+        <f t="shared" ref="H7:H12" si="0">"0"&amp;603</f>
         <v>0603</v>
       </c>
       <c r="I7" t="s">
@@ -814,7 +838,7 @@
         <v>34</v>
       </c>
       <c r="H8" t="str">
-        <f>"0"&amp;603</f>
+        <f t="shared" si="0"/>
         <v>0603</v>
       </c>
       <c r="I8" t="s">
@@ -841,7 +865,7 @@
         <v>36</v>
       </c>
       <c r="H9" t="str">
-        <f>"0"&amp;603</f>
+        <f t="shared" si="0"/>
         <v>0603</v>
       </c>
       <c r="I9" t="s">
@@ -868,7 +892,7 @@
         <v>38</v>
       </c>
       <c r="H10" t="str">
-        <f>"0"&amp;603</f>
+        <f t="shared" si="0"/>
         <v>0603</v>
       </c>
       <c r="I10" t="s">
@@ -895,7 +919,7 @@
         <v>40</v>
       </c>
       <c r="H11" t="str">
-        <f>"0"&amp;603</f>
+        <f t="shared" si="0"/>
         <v>0603</v>
       </c>
       <c r="I11" t="s">
@@ -922,7 +946,7 @@
         <v>43</v>
       </c>
       <c r="H12" t="str">
-        <f>"0"&amp;603</f>
+        <f t="shared" si="0"/>
         <v>0603</v>
       </c>
       <c r="I12" t="s">
@@ -949,7 +973,7 @@
         <v>45</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" ref="H13:H15" si="0">"0"&amp;603</f>
+        <f t="shared" ref="H13:H15" si="1">"0"&amp;603</f>
         <v>0603</v>
       </c>
       <c r="I13" t="s">
@@ -976,7 +1000,7 @@
         <v>47</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0603</v>
       </c>
       <c r="I14" t="s">
@@ -1003,7 +1027,7 @@
         <v>49</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0603</v>
       </c>
       <c r="I15" t="s">
@@ -1017,6 +1041,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
       <c r="C16">
         <v>1</v>
       </c>
@@ -1042,6 +1069,9 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
       </c>
       <c r="C17">
         <v>1</v>

</xml_diff>

<commit_message>
Connected OLED pin connector
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver\Documents\GitHub\65-Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695D610D-8A37-4D3D-9445-BA61B9ED9040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67448974-C91F-442C-A498-EE788123E9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{9889003C-2723-49A8-808D-023C4202CB02}"/>
   </bookViews>
@@ -137,57 +137,9 @@
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0.1 uF 16 VDC 10% 0603 X7R AEC-Q200</t>
   </si>
   <si>
-    <t>GRT188C80J475KE01D</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 4.7 uF 6.3 VDC 10% 0603 X6S AEC-Q200</t>
-  </si>
-  <si>
-    <t>GCE188R72A103MA01D</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0.01 uF 100 VDC 20% 0603 X7R AEC-Q200</t>
-  </si>
-  <si>
-    <t>GCM1885C1H101FA16D</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 100 pF 50 VDC 1% 0603 C0G (NP0) AEC-Q200</t>
-  </si>
-  <si>
-    <t>GRJ188R60J106ME11D</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 10 uF 6.3 VDC 20% 0603 X5R</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>RC0603FR-0710KL</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 10 kOhms 100mW 0603 1%</t>
-  </si>
-  <si>
-    <t>AC0603FR-07470RL</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 470 Ohms 100mW 0603 1% AEC-Q200 Standard Power Version</t>
-  </si>
-  <si>
-    <t>AR0603FR-072KL</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 2k Ohms 1/10 W 0603% 1% AEC-Q200</t>
-  </si>
-  <si>
-    <t>RC0603FR-074K7L</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 4.7 kOhms 100mW 0603 1%</t>
-  </si>
-  <si>
     <t>TPOWER</t>
   </si>
   <si>
@@ -225,13 +177,61 @@
   </si>
   <si>
     <t>U3</t>
+  </si>
+  <si>
+    <t>RC0402FR-7D4K7L</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 4.7 kOhms 62.5 mW 0402 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD </t>
+  </si>
+  <si>
+    <t>RC0402JR-7D10KL</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 10 kOhms 62.5 mW 0402 5%</t>
+  </si>
+  <si>
+    <t>RC0402FR-7D2KL</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 2kOhms 1/16W 0402 1%</t>
+  </si>
+  <si>
+    <t>RC0402JR-07470RL</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 470 Ohms 62.5mW 0402 5%</t>
+  </si>
+  <si>
+    <t>GRM1555C2A101GA01D</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 100 pF 100 VDC 2% 0402 C0G (NP0)</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0402 10uF 4VDC 20% X6S AEC-Q200</t>
+  </si>
+  <si>
+    <t>GRM155R71C103KA01J</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0.01 uF 16 VDC 10% 0402 X7R</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 4.7 uF 6.3 VDC 20% 0402 X5R</t>
+  </si>
+  <si>
+    <t>GRM155R60J475ME47J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +244,12 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14FE901-52FF-4CE6-9C79-25A63A496803}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -692,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -767,7 +773,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -811,7 +817,7 @@
         <v>32</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H12" si="0">"0"&amp;603</f>
+        <f t="shared" ref="H7" si="0">"0"&amp;603</f>
         <v>0603</v>
       </c>
       <c r="I7" t="s">
@@ -832,20 +838,20 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
+        <v>62</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>0603</v>
+        <f t="shared" ref="H8:H9" si="1">"0"&amp;402</f>
+        <v>0402</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -858,21 +864,21 @@
       <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
+      <c r="F9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>0603</v>
+        <f t="shared" si="1"/>
+        <v>0402</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -885,21 +891,21 @@
       <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>38</v>
+      <c r="F10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>0603</v>
+        <f>"0"&amp;402</f>
+        <v>0402</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -912,21 +918,21 @@
       <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>40</v>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>0603</v>
+        <f>"0"&amp;402</f>
+        <v>0402</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -934,26 +940,26 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>0603</v>
+        <f>"0"&amp;402</f>
+        <v>0402</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -961,26 +967,26 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" ref="H13:H15" si="1">"0"&amp;603</f>
-        <v>0603</v>
+        <f>"0"&amp;402</f>
+        <v>0402</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -988,26 +994,26 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="1"/>
-        <v>0603</v>
+        <f t="shared" ref="H14:H15" si="2">"0"&amp;402</f>
+        <v>0402</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1015,26 +1021,26 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>0402</v>
+      </c>
+      <c r="I15" t="s">
         <v>49</v>
       </c>
-      <c r="H15" t="str">
-        <f t="shared" si="1"/>
-        <v>0603</v>
-      </c>
-      <c r="I15" t="s">
-        <v>18</v>
-      </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1042,22 +1048,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1071,25 +1077,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
@@ -1098,8 +1104,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1" display="https://www.mouser.com/ProductDetail/YAGEO/RC0402FR-7D4K7L?qs=F5EMLAvA7ID7%2FFIVczkChg%3D%3D" xr:uid="{C925B2DD-194A-4737-9372-5384CD7E16B7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New Charger IC, Added Ground Plane
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver\Documents\GitHub\65-Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67448974-C91F-442C-A498-EE788123E9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FA5011-E09C-4BD5-9054-CCD44B434152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{9889003C-2723-49A8-808D-023C4202CB02}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Item #</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Include in PCB</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>LQFP-64</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>ARM Microcontrollers - MCU 32BIT Cortex M3 H/D Performance LINE</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>Multiprotocol Modules SMD module, ESP32-S3FN8, 8 MB SPI flash, PCB antenna</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>SMD</t>
   </si>
   <si>
@@ -140,18 +131,6 @@
     <t>Yageo</t>
   </si>
   <si>
-    <t>TPOWER</t>
-  </si>
-  <si>
-    <t>TP4056</t>
-  </si>
-  <si>
-    <t>4V~6V Lithium-ion/Polymer 1 1A ESOP-8 Battery Management ROHS</t>
-  </si>
-  <si>
-    <t>ESOP-8</t>
-  </si>
-  <si>
     <t>MAX17048G+T10</t>
   </si>
   <si>
@@ -225,6 +204,21 @@
   </si>
   <si>
     <t>GRM155R60J475ME47J</t>
+  </si>
+  <si>
+    <t>3PEAK</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>TPB4056B2X-ES1R</t>
+  </si>
+  <si>
+    <t>Charger IC Lithium Ion/Polymer 8-ESOP</t>
+  </si>
+  <si>
+    <t>ESOP8</t>
   </si>
 </sst>
 </file>
@@ -609,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14FE901-52FF-4CE6-9C79-25A63A496803}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,10 +620,9 @@
     <col min="7" max="7" width="79.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -657,72 +650,63 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
       <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
       <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -730,25 +714,22 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>5099</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -756,355 +737,319 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
       <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
       <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" ref="H7" si="0">"0"&amp;603</f>
         <v>0603</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" ref="H8:H9" si="1">"0"&amp;402</f>
         <v>0402</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="1"/>
         <v>0402</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H10" t="str">
         <f>"0"&amp;402</f>
         <v>0402</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H11" t="str">
         <f>"0"&amp;402</f>
         <v>0402</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H12" t="str">
         <f>"0"&amp;402</f>
         <v>0402</v>
       </c>
       <c r="I12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H13" t="str">
         <f>"0"&amp;402</f>
         <v>0402</v>
       </c>
       <c r="I13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" ref="H14:H15" si="2">"0"&amp;402</f>
         <v>0402</v>
       </c>
       <c r="I14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="2"/>
         <v>0402</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Changed gasket mounts and added keepout zone for esp32
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver\Documents\GitHub\65-Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6401C754-C19A-4FA2-92EE-FD0DD1CDC0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4AD1D4-7525-4220-8AFB-B617F8E235BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{9889003C-2723-49A8-808D-023C4202CB02}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9889003C-2723-49A8-808D-023C4202CB02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="134">
   <si>
     <t>Item #</t>
   </si>
@@ -140,18 +140,12 @@
     <t>GRM155R60J475ME47J</t>
   </si>
   <si>
-    <t>TPB4056B2X-ES1R</t>
-  </si>
-  <si>
     <t>https://www.st.com/resource/en/datasheet/stm32f103re.pdf</t>
   </si>
   <si>
     <t>STM32F103RETx</t>
   </si>
   <si>
-    <t>TPB4056A20-ES1R</t>
-  </si>
-  <si>
     <t>https://www.espressif.com/sites/default/files/documentation/esp32-s3-mini-1_mini-1u_datasheet_en.pdf</t>
   </si>
   <si>
@@ -206,18 +200,6 @@
     <t>S1,S2,S3,S4,S5,S6,S7,S8,S9,S10,S11,S12,S13,S14,S16,S17,S18,S19,S20,S21,S22,S23,S24,S25,S26,S27,S31,S32,S33,S34,S35,S36,S37,S38,S39,S40,S41,S42,S43,S44,S45,S46,S47,S48,S49,S50,S51,S52,S53,S54,S56,S57,S61,S64,S65,S66,S71,S72</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>1.2k</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -227,9 +209,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>R1,R3,R5,R11,R12</t>
-  </si>
-  <si>
     <t>https://cdn-shop.adafruit.com/product-files/2686/SK6812MINI_REV.01-1-2.pdf</t>
   </si>
   <si>
@@ -290,12 +269,6 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>C6,C7,C10,C15</t>
-  </si>
-  <si>
-    <t>C1,C2,C3,C4,C5,C9</t>
-  </si>
-  <si>
     <t>Datasheet</t>
   </si>
   <si>
@@ -347,12 +320,6 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>3Peak</t>
-  </si>
-  <si>
-    <t>LINEAR BATTERY CHARGER 1 CELL 8-</t>
-  </si>
-  <si>
     <t>EspressIf</t>
   </si>
   <si>
@@ -371,18 +338,6 @@
     <t>YAGEO</t>
   </si>
   <si>
-    <t>AA0402JR-071K2L</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 1.2kOhms 1/16W 0402 5% AEC-Q200</t>
-  </si>
-  <si>
-    <t>AC0402JR-07100KL</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 100k Ohm 62.5mW 0402 5% AEC-Q200 Standard Power Version</t>
-  </si>
-  <si>
     <t>Cannonkeys</t>
   </si>
   <si>
@@ -426,13 +381,70 @@
   </si>
   <si>
     <t>Logitech MX Master 3s Side Scroll Component</t>
+  </si>
+  <si>
+    <t>C1, C11, C2, C3, C4, C5, C9</t>
+  </si>
+  <si>
+    <t>C10,C15</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>BQ25185DLHR</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>R1, R11, R12, R17, R3, R5</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>UMW</t>
+  </si>
+  <si>
+    <t>3.3V LDO Regulator</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>GXT155R60J105KE01D</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0402 6.3VDC 1uF 10% X5R AEC-Q200</t>
+  </si>
+  <si>
+    <t>MF-FSMF050X-2</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>Resettable Fuses - PPTC 6V .5A-HD 40A MAX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,13 +458,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -467,8 +491,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14FE901-52FF-4CE6-9C79-25A63A496803}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -844,7 +871,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -853,7 +880,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -861,22 +888,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -885,7 +912,7 @@
         <v>402</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -893,22 +920,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
         <v>32</v>
@@ -917,7 +944,7 @@
         <v>402</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -925,22 +952,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -949,7 +976,7 @@
         <v>402</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -957,22 +984,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
         <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
@@ -981,7 +1008,7 @@
         <v>402</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -989,63 +1016,60 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I6">
         <v>402</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" t="s">
-        <v>89</v>
+      <c r="B7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="I7">
-        <v>603</v>
-      </c>
-      <c r="J7" t="s">
-        <v>44</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1053,22 +1077,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>67</v>
       </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>80</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>603</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1076,19 +1109,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1096,19 +1132,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1116,19 +1152,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1136,19 +1172,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C12">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1156,31 +1192,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13">
-        <v>402</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1188,31 +1212,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I14">
         <v>402</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1220,86 +1244,83 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="I15">
         <v>402</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" t="s">
-        <v>114</v>
-      </c>
-      <c r="I16">
+      <c r="B16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="1">
         <v>402</v>
       </c>
-      <c r="J16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17">
-        <v>58</v>
-      </c>
-      <c r="E17" t="s">
-        <v>115</v>
-      </c>
-      <c r="G17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" t="s">
-        <v>44</v>
+      <c r="B17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="1">
+        <v>750</v>
+      </c>
+      <c r="I17" s="1">
+        <v>402</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1307,16 +1328,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
+        <v>12</v>
       </c>
       <c r="J18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1324,16 +1351,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1341,16 +1368,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1361,16 +1388,13 @@
         <v>50</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>117</v>
+        <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" t="s">
-        <v>116</v>
+        <v>49</v>
+      </c>
+      <c r="J21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1378,13 +1402,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="H22" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1392,13 +1422,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1409,25 +1439,10 @@
         <v>46</v>
       </c>
       <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="G24" t="s">
         <v>45</v>
-      </c>
-      <c r="H24" t="s">
-        <v>108</v>
-      </c>
-      <c r="J24" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1435,25 +1450,28 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>90</v>
       </c>
       <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" t="s">
         <v>89</v>
-      </c>
-      <c r="F25" t="s">
-        <v>17</v>
       </c>
       <c r="G25" t="s">
         <v>43</v>
       </c>
       <c r="H25" t="s">
-        <v>107</v>
+        <v>97</v>
+      </c>
+      <c r="J25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1461,28 +1479,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="G26" t="s">
         <v>41</v>
       </c>
       <c r="H26" t="s">
-        <v>106</v>
-      </c>
-      <c r="J26" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1490,7 +1505,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1499,16 +1514,19 @@
         <v>91</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="G27" t="s">
         <v>39</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>95</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1516,28 +1534,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="H28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1545,105 +1560,129 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" t="s">
-        <v>35</v>
+      <c r="B30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
       <c r="C31">
         <v>1</v>
       </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
       <c r="E31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G31" t="s">
-        <v>118</v>
-      </c>
-      <c r="H31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>97</v>
-      </c>
-      <c r="G32" t="s">
-        <v>121</v>
-      </c>
-      <c r="H32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="G32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" t="s">
-        <v>115</v>
-      </c>
-      <c r="H33" t="s">
-        <v>122</v>
+      <c r="B33" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1653,17 +1692,14 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" t="s">
-        <v>124</v>
-      </c>
       <c r="E34" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="G34" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="H34" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,21 +1709,75 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" t="s">
-        <v>128</v>
-      </c>
       <c r="E35" t="s">
-        <v>97</v>
+        <v>88</v>
+      </c>
+      <c r="G35" t="s">
+        <v>106</v>
       </c>
       <c r="H35" t="s">
-        <v>129</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" t="s">
+        <v>100</v>
+      </c>
+      <c r="H36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" t="s">
+        <v>111</v>
+      </c>
+      <c r="H37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1" display="https://www.mouser.com/ProductDetail/YAGEO/RC0402FR-7D4K7L?qs=F5EMLAvA7ID7%2FFIVczkChg%3D%3D" xr:uid="{C925B2DD-194A-4737-9372-5384CD7E16B7}"/>
-    <hyperlink ref="D25" r:id="rId2" display="https://www.mouser.com/manufacturer/maxim-integrated/" xr:uid="{2AFAE00C-9C63-4F5E-B803-C2859BD5AB5C}"/>
+    <hyperlink ref="F15" r:id="rId1" display="https://www.mouser.com/ProductDetail/YAGEO/RC0402FR-7D4K7L?qs=F5EMLAvA7ID7%2FFIVczkChg%3D%3D" xr:uid="{C925B2DD-194A-4737-9372-5384CD7E16B7}"/>
+    <hyperlink ref="D26" r:id="rId2" display="https://www.mouser.com/manufacturer/maxim-integrated/" xr:uid="{2AFAE00C-9C63-4F5E-B803-C2859BD5AB5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>